<commit_message>
Added radio transmission/serial read dummy files
Added radio test and dummy serialread file. Added Gannt Chart and Bumper
circuit diagram.
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="13605"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17760" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,11 +543,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CN22" sqref="CN22"/>
+      <selection activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +628,16 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" t="s">

</xml_diff>